<commit_message>
Added DB Activities package
</commit_message>
<xml_diff>
--- a/SourceCode/2023/July2023/Rajasekhar/RPA Challenge_REFramework/Data/Config.xlsx
+++ b/SourceCode/2023/July2023/Rajasekhar/RPA Challenge_REFramework/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sekha\Documents\GitHub\RPA-Developer-in-30-Days\SourceCode\2023\July2023\Rajasekhar\RPA Challenge_REFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D24092-8344-47E5-AC3A-89A26D2A8B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA740BD-68C0-4B9F-9318-EE981E6B6BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -98,81 +98,95 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>StorageBucketName</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
-    <t>Filename</t>
-  </si>
-  <si>
-    <t>Challenge.xlsx</t>
+  </si>
+  <si>
+    <t>StoragePath</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Rajasekhar</t>
+  </si>
+  <si>
+    <t>RpaChallenge</t>
+  </si>
+  <si>
+    <t>challenge.xlsx</t>
+  </si>
+  <si>
+    <t>Challenge1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -196,6 +210,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -217,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -227,6 +247,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +565,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -591,10 +612,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -602,11 +623,13 @@
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -623,14 +646,28 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s">
-        <v>46</v>
+      <c r="B8" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1686,18 +1723,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1721,7 +1758,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1743,7 +1780,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1754,7 +1791,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1765,53 +1802,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2813,7 +2850,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>